<commit_message>
Summery DTO Referencing for fix the cycle loop error
</commit_message>
<xml_diff>
--- a/PendingWorkItems.xlsx
+++ b/PendingWorkItems.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PersonalApplications\MunicipalLKByGLPSolutions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PersonalApplications\OfficeCoPilotV2\MunicipalLKByGLPSolutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742B56DE-3068-432E-B43D-F9430BC93337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B841398-5B37-487B-93A8-EBCA54AB7CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2760" yWindow="3165" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Type</t>
   </si>
@@ -55,6 +58,9 @@
   </si>
   <si>
     <t>When getting building and permit application list , need to do proper paging to reduce load</t>
+  </si>
+  <si>
+    <t>Plan Application Main Grid , filters , sort , search not working</t>
   </si>
 </sst>
 </file>
@@ -385,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,6 +470,17 @@
         <v>45916</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2">
+        <v>45946</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Assign to committee final changes , the navigations and saving
</commit_message>
<xml_diff>
--- a/PendingWorkItems.xlsx
+++ b/PendingWorkItems.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PersonalApplications\OfficeCoPilotV2\MunicipalLKByGLPSolutions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MuniLogicApplications\MunicipalLKByGLPSolutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B841398-5B37-487B-93A8-EBCA54AB7CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A3446E-48C0-4B8B-B704-9425E4286F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="3165" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Type</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Plan Application Main Grid , filters , sort , search not working</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>Check migration EF , if its properly creating the planning meeting members and reviews relationship columns</t>
   </si>
 </sst>
 </file>
@@ -391,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,6 +487,17 @@
         <v>45946</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2">
+        <v>45971</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>